<commit_message>
connected categorylist to different yoga post
</commit_message>
<xml_diff>
--- a/Yoga App - WinForm Application/YogaApp/Files/PoseData.xlsx
+++ b/Yoga App - WinForm Application/YogaApp/Files/PoseData.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Project\YogaApp\Yoga App - WinForm Application\YogaApp\Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t>name</t>
   </si>
@@ -39,16 +39,56 @@
   </si>
   <si>
     <t>pathak</t>
+  </si>
+  <si>
+    <t>\\Videos\\TreePose.mp4</t>
+  </si>
+  <si>
+    <t>TreePoseVideoPath</t>
+  </si>
+  <si>
+    <t>TreePoseVideoDescription</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tree Pose or Vrksasana
+ • From standing pose, shift your weight on to the left leg. Ground your left foot down into the floor, pull up your knee cap and thigh.
+• Gaze at a point on eye level, to help you balance.
+• Bend your right knee, reach down with your right hand and clasp your ankle.
+• With help of the hand, place your right foot on the inside of the left leg, if its available to you on the inner thigh, with your heel up high. Lengthen your tailbone toward the floor.
+• If that is not available to you, place the inside of the foot on the inside of the ankle or calf. Avoid the inside of the knee.
+• Turn the knee out to the side, press your foot against the inner thigh, and the inner thigh back into the foot.
+• Bring your hands in front of your heart in prayer position, or you can lift your arms up to the ceiling. hands shoulderwidth apart.
+• With arms lifted, lift from the back body.
+• Stay in this pose for about 30 sec or 1 min.
+• On an outbreath lower the leg and arms down and stand straight, repeat on the other side.
+BENEFITS:
+• Improves balance
+• Opens the hips
+• Strengthens the ankles, legs and spine
+• Lengthens the spine
+• Improves focus/ concentration
+Things to keep in Mind:
+• Make sure you keep both arm extended.
+• Try to avoid collapsing the side body - keep your chest expanded.
+</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -71,13 +111,19 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -356,10 +402,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:B5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -392,7 +438,26 @@
         <v>4</v>
       </c>
     </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" ht="409.5" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>7</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B4" r:id="rId1"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
updating excel file and fixing info display functionality
</commit_message>
<xml_diff>
--- a/Yoga App - WinForm Application/YogaApp/Files/PoseData.xlsx
+++ b/Yoga App - WinForm Application/YogaApp/Files/PoseData.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Project\YogaApp\Yoga App - WinForm Application\YogaApp\Files\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\tholos.itserv.scss.tcd.ie\Pgrad\pathaks\Desktop\YogaApp\Yoga App - WinForm Application\YogaApp\Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25200" windowHeight="11985"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="18870" windowHeight="7815"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,22 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
-  <si>
-    <t>name</t>
-  </si>
-  <si>
-    <t>saurabh</t>
-  </si>
-  <si>
-    <t>age</t>
-  </si>
-  <si>
-    <t>surname</t>
-  </si>
-  <si>
-    <t>pathak</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
     <t>\\Videos\\TreePose.mp4</t>
   </si>
@@ -402,10 +387,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B5"/>
+  <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -416,47 +401,23 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>2</v>
       </c>
-      <c r="B2">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+      <c r="B2" s="2" t="s">
         <v>3</v>
-      </c>
-      <c r="B3" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>6</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" ht="409.5" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>7</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>8</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B4" r:id="rId1"/>
+    <hyperlink ref="B1" r:id="rId1"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
adding category wise pose data
</commit_message>
<xml_diff>
--- a/Yoga App - WinForm Application/YogaApp/Files/PoseData.xlsx
+++ b/Yoga App - WinForm Application/YogaApp/Files/PoseData.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t>\\Videos\\TreePose.mp4</t>
   </si>
@@ -56,6 +56,30 @@
 • Make sure you keep both arm extended.
 • Try to avoid collapsing the side body - keep your chest expanded.
 </t>
+  </si>
+  <si>
+    <t>Beginner</t>
+  </si>
+  <si>
+    <t>Tree Pose 1,Tree Pose 2</t>
+  </si>
+  <si>
+    <t>Intermediate</t>
+  </si>
+  <si>
+    <t>Advanced</t>
+  </si>
+  <si>
+    <t>Expert</t>
+  </si>
+  <si>
+    <t>Tree Pose 3,Tree Pose 4</t>
+  </si>
+  <si>
+    <t>Tree Pose 5,Tree Pose 6</t>
+  </si>
+  <si>
+    <t>Tree Pose 7,Tree Pose 8</t>
   </si>
 </sst>
 </file>
@@ -387,10 +411,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+      <selection activeCell="M6" sqref="M6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -401,23 +425,55 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B5" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="409.5" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+    <row r="6" spans="1:2" ht="409.5" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B6" s="2" t="s">
         <v>3</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B1" r:id="rId1"/>
+    <hyperlink ref="B5" r:id="rId1"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
added function to choose yoga post automaticlly and added other Yoga catpost
</commit_message>
<xml_diff>
--- a/Yoga App - WinForm Application/YogaApp/Files/PoseData.xlsx
+++ b/Yoga App - WinForm Application/YogaApp/Files/PoseData.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\tholos.itserv.scss.tcd.ie\Pgrad\pathaks\Desktop\YogaApp\Yoga App - WinForm Application\YogaApp\Files\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Project\YogaApp\Yoga App - WinForm Application\YogaApp\Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
   <si>
     <t>\\Videos\\TreePose.mp4</t>
   </si>
@@ -80,6 +80,36 @@
   </si>
   <si>
     <t>Tree Pose 7,Tree Pose 8</t>
+  </si>
+  <si>
+    <t>CatPoseVideoPose</t>
+  </si>
+  <si>
+    <t>\\Videos\\CatPose.mp4</t>
+  </si>
+  <si>
+    <t>CatPoseVideoDescription</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Majaryasana or Cat Pose
+• Start on your hands and knees (all fours). Knees directly under hips and wrists, elbows and shoulders in line with each other. Neck in line with your spine, gaze resting softly on the floor.
+• Spread your fingers and press through the base of the fingers and the finger tips.
+• Exhale and round your spine towards the ceiling, lifting the side waists.
+• Pull in your abdominals and tuck your tailbone, gently contracting your glutes. Try to keep your shoulders and knees in position.
+• Release your head towards the floor and press firmly into your hands.
+• Inhale and come back into your neutral starting position.
+BENEFITS:
+• Stretches the back and neck.
+• Gently massages the spine, increasing mobility.
+• A great warm up before yoga practice.
+• Helps relieve stress.
+• Increases circulation of spinal fluid.
+• Massages your digestive organs.
+• Stimulates blood circulation in the wrists, especially helpful after a lot of computer work.
+Things to keep in mind:
+• If you have a neck injury, keep your head in the neutral position.
+• Pose should be avoided if you have recent wrist or knee injuries. Instead you can practice a seated or lying down version of Cat - Cow.
+</t>
   </si>
 </sst>
 </file>
@@ -411,10 +441,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B6"/>
+  <dimension ref="A1:B8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M6" sqref="M6"/>
+    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -471,9 +501,26 @@
         <v>3</v>
       </c>
     </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>12</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" ht="409.5" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>14</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="B5" r:id="rId1"/>
+    <hyperlink ref="B7" r:id="rId2"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
fixing path variable in excel and refactoring code
</commit_message>
<xml_diff>
--- a/Yoga App - WinForm Application/YogaApp/Files/PoseData.xlsx
+++ b/Yoga App - WinForm Application/YogaApp/Files/PoseData.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Project\YogaApp\Yoga App - WinForm Application\YogaApp\Files\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\tholos.itserv.scss.tcd.ie\Pgrad\pathaks\Desktop\YogaApp\Yoga App - WinForm Application\YogaApp\Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -82,9 +82,6 @@
     <t>Tree Pose 7,Tree Pose 8</t>
   </si>
   <si>
-    <t>CatPoseVideoPose</t>
-  </si>
-  <si>
     <t>\\Videos\\CatPose.mp4</t>
   </si>
   <si>
@@ -110,6 +107,9 @@
 • If you have a neck injury, keep your head in the neutral position.
 • Pose should be avoided if you have recent wrist or knee injuries. Instead you can practice a seated or lying down version of Cat - Cow.
 </t>
+  </si>
+  <si>
+    <t>CatPoseVideoPath</t>
   </si>
 </sst>
 </file>
@@ -443,8 +443,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B8"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -503,18 +503,18 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
+        <v>15</v>
+      </c>
+      <c r="B7" s="1" t="s">
         <v>12</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>13</v>
       </c>
     </row>
     <row r="8" spans="1:2" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
+        <v>13</v>
+      </c>
+      <c r="B8" s="2" t="s">
         <v>14</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>15</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
adding implementation for dynamically adding buttons to form
</commit_message>
<xml_diff>
--- a/Yoga App - WinForm Application/YogaApp/Files/PoseData.xlsx
+++ b/Yoga App - WinForm Application/YogaApp/Files/PoseData.xlsx
@@ -61,9 +61,6 @@
     <t>Beginner</t>
   </si>
   <si>
-    <t>Tree Pose 1,Tree Pose 2</t>
-  </si>
-  <si>
     <t>Intermediate</t>
   </si>
   <si>
@@ -110,6 +107,9 @@
   </si>
   <si>
     <t>CatPoseVideoPath</t>
+  </si>
+  <si>
+    <t>Tree Pose:TreePose,Cat Pose:CatPose</t>
   </si>
 </sst>
 </file>
@@ -443,14 +443,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B8"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="28.42578125" customWidth="1"/>
-    <col min="2" max="2" width="28.28515625" customWidth="1"/>
+    <col min="2" max="2" width="39.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
@@ -458,31 +458,31 @@
         <v>4</v>
       </c>
       <c r="B1" t="s">
-        <v>5</v>
+        <v>15</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
@@ -503,18 +503,18 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="8" spans="1:2" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
+        <v>12</v>
+      </c>
+      <c r="B8" s="2" t="s">
         <v>13</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>14</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
adding all the poses to the ui
</commit_message>
<xml_diff>
--- a/Yoga App - WinForm Application/YogaApp/Files/PoseData.xlsx
+++ b/Yoga App - WinForm Application/YogaApp/Files/PoseData.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="40">
   <si>
     <t>\\Videos\\TreePose.mp4</t>
   </si>
@@ -35,7 +35,232 @@
     <t>TreePoseVideoDescription</t>
   </si>
   <si>
+    <t>Beginner</t>
+  </si>
+  <si>
+    <t>Intermediate</t>
+  </si>
+  <si>
+    <t>Advanced</t>
+  </si>
+  <si>
+    <t>Expert</t>
+  </si>
+  <si>
+    <t>\\Videos\\CatPose.mp4</t>
+  </si>
+  <si>
+    <t>CatPoseVideoDescription</t>
+  </si>
+  <si>
+    <t>CatPoseVideoPath</t>
+  </si>
+  <si>
+    <t>Tree Pose:TreePose,Cat Pose:CatPose</t>
+  </si>
+  <si>
+    <t>Bow Pose:BowPose,Bridge Pose:BridgePose</t>
+  </si>
+  <si>
+    <t>Camel Pose:CamelPose,Chair Pose:ChairPose</t>
+  </si>
+  <si>
+    <t>Cow Pose:CowPose,Triangle Pose:TrianglePose</t>
+  </si>
+  <si>
+    <t>BowPoseVideoPath</t>
+  </si>
+  <si>
+    <t>BowPoseVideoDescription</t>
+  </si>
+  <si>
+    <t>\\Videos\\BowPose.mp4</t>
+  </si>
+  <si>
+    <t>BridgePoseVideoPath</t>
+  </si>
+  <si>
+    <t>BridgePoseVideoDescription</t>
+  </si>
+  <si>
+    <t>\\Videos\\BridgePose.mp4</t>
+  </si>
+  <si>
+    <t>CamelPoseVideoPath</t>
+  </si>
+  <si>
+    <t>CamelPoseVideoDescription</t>
+  </si>
+  <si>
+    <t>\\Videos\\CamelPose.mp4</t>
+  </si>
+  <si>
+    <t>ChairPoseVideoPath</t>
+  </si>
+  <si>
+    <t>ChairPoseVideoDescription</t>
+  </si>
+  <si>
+    <t>\\Videos\\ChairPose.mp4</t>
+  </si>
+  <si>
+    <t>CowPoseVideoPath</t>
+  </si>
+  <si>
+    <t>CowPoseVideoDescription</t>
+  </si>
+  <si>
+    <t>\\Videos\\CowPose.mp4</t>
+  </si>
+  <si>
+    <t>TrianglePoseVideoPath</t>
+  </si>
+  <si>
+    <t>TrianglePoseVideoDescription</t>
+  </si>
+  <si>
+    <t>\\Videos\\TrianglePose.mp4</t>
+  </si>
+  <si>
+    <t>Dhanurasana or Bow Pose
+STEPS:
+Lie on your stomach with your hands by your torso, palms up.
+Exhale and bend your knees, bringing your feet as close as you can to your buttocks and grab the ankles with your hands.
+Inhale press the pubic bone down, pull the belly in and push the ankles against the hands as you pull with the arms. Lifting the thighs and the chest.
+Press your shoulder blades into your back to open the heart.
+Stay here for a few breaths, breathing into your back body (this position can make it quite difficult to breathe fully).
+On an exhale release your arms, core engaged and come gently lying in a prone position. Lie quietly for a few breaths.
+BENEFITS:
+Strengthens the back
+Opens the chest
+Helps stretch the front body
+Energizing
+Helps ease anxiety
+Stimulates organs
+Things to keep in mind:
+Make sure that your knees are not wider than the width of your hips.
+If you feel tension in your neck, drop your chin towards your chest.
+If you have blood pressure issues, recurring headaches or back injury this pose should be avoided.</t>
+  </si>
+  <si>
+    <t>Setu Bandha Sarvangasana or Bridge Pose
+STEPS:
+Lie on your back with your arms next to the body, palms down.
+Bend your knees and place your feet flat on the floor, heels close to the buttocks, hip width apart.
+With the feet parallel to each other, press the upper arms into the floor, press your feet into the floor (inside and outside equally) and begin to lift the hips up to the ceiling, moving your breastbone to the chin, but not the chin to the breastbone.  +Lift your chin slightly to keep space under the back of the neck. 
+Firm your tailbone in towards the pubic bone and your pubic bone moves slightly towards the belly. +
+Actively bring the knees out in front of you to keep the lower back extended. Keep the knees above the ankles.
+Your buttocks are firm but not clenched. + Your hips are lifted as high as is available to you with these principles in place.  +
+Clasp your hands behind the back and firm the arms into the floor, shoulder blades are down along the spine. 
+You can take between 5 and 15 breaths in this pose. +
+To come out, release the arms and lower the hips down to the floor on an out-breath.
+BENEFITS:
+Stretches chest and spine.
+Strengthens legs, glutes and upper back.
+Improves digestion.
+Reduces backache and headache.
+Calms the mind, improves the mood.
+Can help to open the sinuses.
+Things to keep in mind:
+Your neck - as your raise up higher make sure you don't flatten the back of the neck into the ground. If you have a neck injury avoid this pose unless you are being supervised by a professional.
+Your feet - make sure your feet are parallel with each other and try not to let your knees fall away from each other.</t>
+  </si>
+  <si>
+    <t>Ustrasana or Camel Pose
+STEPS:
+Come on your knees, place the knees hip width apart, body upright. Toes tucked under, or if you are more flexible, point your toes back.
+Place your hands on your lower back, heels of the hands resting on the lower back, fingers pointing down.
+Engage your legs. Pull the thighs back so the hips are still over the knees. Rotate the inner thighs in a little and with your hands help to lengthen the buttocks down. At the same time visualise drawing the front hipbones together and up to activate the belly. Your hip bones and lower ribs firm towards each other. Try to maintain this action throughout the pose.
+With the lower body stable, begin to breathe in towards the chest, drawing the shoulder blades back as you lift the chest.
+On an exhale start to come into your backbend keeping the chest lifted and without crunching the neck or lower back.
+You can keep the head neutral throughout the pose, chin towards the sternum (recommended), if you take the head back, do so only when the opening in the chest is at its fullest and your neck is long and happy.
+Lift the lower back ribs away from the lumbar spine to create even more length in the lower back and to facilitate the opening in the chest even more.
+Stay in this pose anywhere from 30 seconds to a minute, breathing into the chest to facilitate the opening there. When you notice you cannot breathe properly you are taking the pose too far and you should back off to a variation you can sustain with breathing smoothly.
+To come out, place the hands to the front hip bones and guide them down as you lift back up on an inhalation. If your head is all the way back lead with the heart, bring the head up last.
+Neutralize and lengthen your spine in Downward Facing Dog Pose before resting in Child's Pose for a few breaths.
+BENEFITS:
+Opens the belly, chest, heart, shoulders and upper back.
+Stretches the whole front of the body including ankles, thighs and groin.
+Strengthens the legs and back.
+Improves your posture.
+Stimulates the organs in the belly.
+Energizes body and mind.
+Things to keep in mind:
+Straining your neck - if you have any injury or neck sensitivity please keep your neck in a neutral position or with the chin towards the chest so that the back of the neck is long and relaxed.
+Lower back - if you have a back injury do a more gentle backbend like the sphinx pose.
+Lightheadedness / dizziness - if you are compressing the neck too much it can lead to these sensations. 
+Sensitive knees - place a blanket or double your mat under your knees to reduce sensitivity.</t>
+  </si>
+  <si>
+    <t>Utkatasana or Chair Pose
+STEPS:
+Stand with your feet together, base of big toes touching, heels slightly apart, or with your feet hip distance apart.
+Exhale as you bend the knees as if you’re about to sit down on a chair. Bring your thighs as close to parallel with the floor as possible. Send your hips back rather than your knees forward, so that you can still see your toes.
+Keep the back straight as you lean forward from the hips slightly.
+Inhale as you raise your arms up in line with your ears or in front of them.
+Keep the neck long, slide your shoulder blades down and firm them into the back.
+Pull your lower abdomen in and up, this helps to extend and protect the lower back.
+Stay in Utkatasana from 5 to 15 breaths.
+To come out of the pose, inhale, press into your feet and straighten the legs, reaching up through the fingers and the crown of your head. Exhale and lower your arms to come back into starting pose.
+BENEFITS:
+Strengthens and stabilises the legs, ankles and feet.
+Strengthens the abdominal muscles and lower back.
+Opens and stretches the chest and shoulders.
+Improves confidence and focus.
+Great pose to practice Mula Bandha and Uddiyana Bandha which will create lightness and also tones the pelvic floor muscles and lower abdomen.
+Things to keep in mind:
+Protect your knees: Double check that they don’t come forward over the line of the toes. You should be able to see the toes.
+If you have discomfort in your shoulders or neck, bring your arms wider apart and/or lower. They can be pointing straight out in front of you or down to the floor. Alternatively you could bend the elbows in line with the ears and point the fingertips upwards.
+Lower back: Ensure that your lower belly is drawn back to the spine to protect your lower back, try not to overarch the lumbar spine. If you have back problems either skip the pose or practice with your back against a wall.</t>
+  </si>
+  <si>
+    <t>Bitilasana or Cow Pose
+STEPS:
+Start on hands and knees (all fours) - in a tabletop position. Your knees directly below your hips and you wrists in line with your shoulders. Spread your fingers, middle finger pointing forward. Place your head in a neutral position, your gaze resting softly on the floor.
+Inhale, lift your sitting bones up towards the ceiling. Open your chest and allow your belly to sink towards the floor. Lifting your head to look straight forward or look up (whatever is comfortable for you)
+Exhale, come back into your neutral 'tabletop' position.
+BENEFITS:
+Stretches the front of the torso and neck.
+Helps relieve stress.
+Massages the spine and internal organs.
+Great as a warm up before class along with other spinal movements like Cat pose.
+Things to keep in mind:
+Protect your neck - drop the shoulders down away from ears. Try not to crunch the back of the neck as you look up.
+Neck injury - keep your head and neck in a neutral position.</t>
+  </si>
+  <si>
+    <t>Utthita Trikonasana or Extended Triangle Pose
+STEPS:
+Facing the long edge of your mat, step your feet wide apart, about the length of your leg.
+Turn your right foot 90 degrees so the toes point to the short edge of the mat, and turn the left foot in about 45 degrees towards the right.
+Distribute weight evenly over the four corners of both feet, lift arches and inner ankles up.
+With straight legs, lift your knee caps drawing the top of thighs up and back, roll the right thigh out so the right knee is in line with first two toes.
+Lengthen through both sides of the waist, draw you lower belly in and up. Inhale and lift your arms parallel to the floor, extend through to the fingertips as you exhale.
+Inhale and reach to the right extending your body over your right leg, shift your hips towards the back of the mat and exhale as you bring your right arm down, placing your hand where it reaches, either on the leg, foot, the floor or a block outside the foot.
+Point the left arm straight up to the ceiling, hand in line with your shoulder, palm facing forwards.
+Keep as much length in the left side waist as in the right, rotate your ribs to the ceiling.
+Lengthen through the sides of the neck, keeping your neck in line with spine. Look straight in front of you, or tuck the chin slightly and turn to look up toward your left hand.
+Keep your face relaxed and breath gently as you keep pressing through the feet, extending through fingertips and lengthening through the crown of the head.
+To come out press your feet firmly into the floor, inhale and reach your left arm up to the ceiling as you come back to standing straight.
+Pivot your heels so you reverse the orientation of your feet to the other side and repeat on the left.
+BENEFITS:
+Strengthens the legs and back.
+Stretches inner thighs, hamstrings, calves, spine, shoulders, chest and opens hips.
+Energizes, balances and focuses you.
+Stimulates abdominal organs.
+Things to keep in mind:
+Your knees. Don't rest your hand directly on your knee as this is too much weight on the joint.
+Locking the knee too much. You can keep a micro-bend in the leg you are bending towards. This will also work your muscles more.
+If you have neck problems - keep the gaze straight ahead or look down to the floor instead of looking to the top hand.</t>
+  </si>
+  <si>
     <t xml:space="preserve">Tree Pose or Vrksasana
+STEPS:
  • From standing pose, shift your weight on to the left leg. Ground your left foot down into the floor, pull up your knee cap and thigh.
 • Gaze at a point on eye level, to help you balance.
 • Bend your right knee, reach down with your right hand and clasp your ankle.
@@ -58,34 +283,8 @@
 </t>
   </si>
   <si>
-    <t>Beginner</t>
-  </si>
-  <si>
-    <t>Intermediate</t>
-  </si>
-  <si>
-    <t>Advanced</t>
-  </si>
-  <si>
-    <t>Expert</t>
-  </si>
-  <si>
-    <t>Tree Pose 3,Tree Pose 4</t>
-  </si>
-  <si>
-    <t>Tree Pose 5,Tree Pose 6</t>
-  </si>
-  <si>
-    <t>Tree Pose 7,Tree Pose 8</t>
-  </si>
-  <si>
-    <t>\\Videos\\CatPose.mp4</t>
-  </si>
-  <si>
-    <t>CatPoseVideoDescription</t>
-  </si>
-  <si>
     <t xml:space="preserve">Majaryasana or Cat Pose
+STEPS:
 • Start on your hands and knees (all fours). Knees directly under hips and wrists, elbows and shoulders in line with each other. Neck in line with your spine, gaze resting softly on the floor.
 • Spread your fingers and press through the base of the fingers and the finger tips.
 • Exhale and round your spine towards the ceiling, lifting the side waists.
@@ -104,12 +303,6 @@
 • If you have a neck injury, keep your head in the neutral position.
 • Pose should be avoided if you have recent wrist or knee injuries. Instead you can practice a seated or lying down version of Cat - Cow.
 </t>
-  </si>
-  <si>
-    <t>CatPoseVideoPath</t>
-  </si>
-  <si>
-    <t>Tree Pose:TreePose,Cat Pose:CatPose</t>
   </si>
 </sst>
 </file>
@@ -441,48 +634,48 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B8"/>
+  <dimension ref="A1:B20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="28.42578125" customWidth="1"/>
-    <col min="2" max="2" width="39.7109375" customWidth="1"/>
+    <col min="2" max="2" width="58.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B1" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B2" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B3" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B4" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
@@ -498,29 +691,131 @@
         <v>2</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>3</v>
+        <v>38</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
     </row>
     <row r="8" spans="1:2" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>13</v>
+        <v>39</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>14</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" ht="409.5" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>15</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>17</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" ht="409.5" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>18</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>20</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" ht="409.5" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>21</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>23</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" ht="409.5" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>24</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>26</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" ht="375" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>27</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>29</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" ht="409.5" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>30</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>37</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="B5" r:id="rId1"/>
     <hyperlink ref="B7" r:id="rId2"/>
+    <hyperlink ref="B9" r:id="rId3"/>
+    <hyperlink ref="B11" r:id="rId4"/>
+    <hyperlink ref="B13" r:id="rId5"/>
+    <hyperlink ref="B15" r:id="rId6"/>
+    <hyperlink ref="B17" r:id="rId7"/>
+    <hyperlink ref="B19" r:id="rId8"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>